<commit_message>
EOD 06/07/2016 - Amend Contract - Suspend and System Mail
Added function waitForElementToVanish to GeneralFunctions
</commit_message>
<xml_diff>
--- a/TestData/Testdata.xlsx
+++ b/TestData/Testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="129">
   <si>
     <t>Execution</t>
   </si>
@@ -392,6 +392,18 @@
   </si>
   <si>
     <t>Test promo 17-2-16</t>
+  </si>
+  <si>
+    <t>cSAmendContract_SystemLetter_START</t>
+  </si>
+  <si>
+    <t>cSAmendContract_SystemLetter_END</t>
+  </si>
+  <si>
+    <t>LetterName</t>
+  </si>
+  <si>
+    <t>No Stock Sub Ext By 1</t>
   </si>
 </sst>
 </file>
@@ -463,7 +475,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -479,6 +491,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -818,15 +831,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V54"/>
+  <dimension ref="A1:V59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
@@ -2042,6 +2055,62 @@
         <v>123</v>
       </c>
     </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B58" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H58" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
@@ -2056,9 +2125,10 @@
     <hyperlink ref="C43" r:id="rId10"/>
     <hyperlink ref="C48" r:id="rId11"/>
     <hyperlink ref="C53" r:id="rId12"/>
+    <hyperlink ref="C58" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
   <ignoredErrors>
     <ignoredError sqref="O3:P3 N8:O8" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
General Functions- Added a function for element highlight
Customer Services - Mailing Method, Change Term, Resume added
</commit_message>
<xml_diff>
--- a/TestData/Testdata.xlsx
+++ b/TestData/Testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="158">
   <si>
     <t>Execution</t>
   </si>
@@ -404,6 +404,93 @@
   </si>
   <si>
     <t>No Stock Sub Ext By 1</t>
+  </si>
+  <si>
+    <t>cSAmendContract_Suspend_START</t>
+  </si>
+  <si>
+    <t>cSAmendContract_Suspend_END</t>
+  </si>
+  <si>
+    <t>DOVECU4347471</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Payment rejected</t>
+  </si>
+  <si>
+    <t>cSAmendContract_Resume_START</t>
+  </si>
+  <si>
+    <t>cSAmendContract_Resume_END</t>
+  </si>
+  <si>
+    <t>Contract Resumption - Finance Authorised</t>
+  </si>
+  <si>
+    <t>AUG-16</t>
+  </si>
+  <si>
+    <t>ResumeStartingFrom</t>
+  </si>
+  <si>
+    <t>cSAmendContract_RefundAmount_START</t>
+  </si>
+  <si>
+    <t>cSAmendContract_RefundAmount_END</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>SFG FSG DFSG</t>
+  </si>
+  <si>
+    <t>BACS Subscriber deceased</t>
+  </si>
+  <si>
+    <t>MailingMethod</t>
+  </si>
+  <si>
+    <t>Surface Mail</t>
+  </si>
+  <si>
+    <t>3.00</t>
+  </si>
+  <si>
+    <t>cSAmendContract_MailingMethod_START</t>
+  </si>
+  <si>
+    <t>cSAmendContract_MailingMethod_END</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>IssueType</t>
+  </si>
+  <si>
+    <t>NumberOfIssues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Term Change - Compensation </t>
+  </si>
+  <si>
+    <t>PAID</t>
+  </si>
+  <si>
+    <t>cSAmendContract_ChangeTerm_START</t>
+  </si>
+  <si>
+    <t>cSAmendContract_ChangeTerm_END</t>
+  </si>
+  <si>
+    <t>DOVECU4347580</t>
+  </si>
+  <si>
+    <t>ADD_ENTITLEMENT</t>
   </si>
 </sst>
 </file>
@@ -475,7 +562,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -492,6 +579,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -831,20 +919,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V59"/>
+  <dimension ref="A1:V84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="C70" workbookViewId="0">
+      <selection activeCell="J83" sqref="J83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.7109375" customWidth="1"/>
     <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="56.42578125" bestFit="1" customWidth="1"/>
@@ -2111,6 +2201,322 @@
         <v>126</v>
       </c>
     </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B62" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B63" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H63" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B67" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B68" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H68" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="I68" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B72" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B73" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I73" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="J73" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B77" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B78" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H78" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B82" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I82" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="J82" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="K82" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B83" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J83" s="10">
+        <v>2</v>
+      </c>
+      <c r="K83" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
@@ -2126,9 +2532,14 @@
     <hyperlink ref="C48" r:id="rId11"/>
     <hyperlink ref="C53" r:id="rId12"/>
     <hyperlink ref="C58" r:id="rId13"/>
+    <hyperlink ref="C63" r:id="rId14"/>
+    <hyperlink ref="C68" r:id="rId15"/>
+    <hyperlink ref="C73" r:id="rId16"/>
+    <hyperlink ref="C78" r:id="rId17"/>
+    <hyperlink ref="C83" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
   <ignoredErrors>
     <ignoredError sqref="O3:P3 N8:O8" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
Account admin  - Product only subscription done
</commit_message>
<xml_diff>
--- a/TestData/Testdata.xlsx
+++ b/TestData/Testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11310" windowHeight="3510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11310" windowHeight="3510" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Service" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="184">
   <si>
     <t>Execution</t>
   </si>
@@ -548,6 +548,27 @@
   </si>
   <si>
     <t>4111111111111111</t>
+  </si>
+  <si>
+    <t>productOnlySchedule_START</t>
+  </si>
+  <si>
+    <t>productOnlySchedule_END</t>
+  </si>
+  <si>
+    <t>PRODUCT_ONLY</t>
+  </si>
+  <si>
+    <t>MERCHANDISE</t>
+  </si>
+  <si>
+    <t>ProductOnly</t>
+  </si>
+  <si>
+    <t>EventDelivery</t>
+  </si>
+  <si>
+    <t>CD Holder - subscriber</t>
   </si>
 </sst>
 </file>
@@ -986,7 +1007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView topLeftCell="M10" workbookViewId="0">
       <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
@@ -2725,10 +2746,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2741,18 +2762,19 @@
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="25" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -2796,7 +2818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>89</v>
       </c>
@@ -2840,17 +2862,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
@@ -2894,7 +2916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>89</v>
       </c>
@@ -2938,15 +2960,126 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
     <hyperlink ref="C8" r:id="rId2"/>
+    <hyperlink ref="C13" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes made in account admin: Back issues - blockers
</commit_message>
<xml_diff>
--- a/TestData/Testdata.xlsx
+++ b/TestData/Testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="194">
   <si>
     <t>Execution</t>
   </si>
@@ -569,6 +569,36 @@
   </si>
   <si>
     <t>CD Holder - subscriber</t>
+  </si>
+  <si>
+    <t>Product Only Schedule</t>
+  </si>
+  <si>
+    <t>Product only Schedule</t>
+  </si>
+  <si>
+    <t>Back Issues Schedule</t>
+  </si>
+  <si>
+    <t>Back Issues</t>
+  </si>
+  <si>
+    <t>IssueDelivery</t>
+  </si>
+  <si>
+    <t>Include Only</t>
+  </si>
+  <si>
+    <t>BackIssues</t>
+  </si>
+  <si>
+    <t>backIssuesSchedule_START</t>
+  </si>
+  <si>
+    <t>backIssuesSchedule_END</t>
+  </si>
+  <si>
+    <t>BACKISSUE</t>
   </si>
 </sst>
 </file>
@@ -647,7 +677,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -666,6 +696,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2746,10 +2777,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3043,10 +3074,10 @@
         <v>33</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>117</v>
+        <v>185</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>38</v>
+        <v>184</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>179</v>
@@ -3073,6 +3104,128 @@
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="R18" s="12">
+        <v>38504</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -3080,6 +3233,7 @@
     <hyperlink ref="C3" r:id="rId1"/>
     <hyperlink ref="C8" r:id="rId2"/>
     <hyperlink ref="C13" r:id="rId3"/>
+    <hyperlink ref="C18" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Renewal Strategy, Account Admin change to schedule
</commit_message>
<xml_diff>
--- a/TestData/Testdata.xlsx
+++ b/TestData/Testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="214">
   <si>
     <t>Execution</t>
   </si>
@@ -599,6 +599,66 @@
   </si>
   <si>
     <t>BACKISSUE</t>
+  </si>
+  <si>
+    <t>JUN 05</t>
+  </si>
+  <si>
+    <t>Schedule</t>
+  </si>
+  <si>
+    <t>UK CWO-DOVEBR6</t>
+  </si>
+  <si>
+    <t>maintSchedule_START</t>
+  </si>
+  <si>
+    <t>maintSchedule_END</t>
+  </si>
+  <si>
+    <t>UK CWO-DOVEBR6-Edited</t>
+  </si>
+  <si>
+    <t>NewDesc</t>
+  </si>
+  <si>
+    <t>Edited</t>
+  </si>
+  <si>
+    <t>cARenewalStartegy_START</t>
+  </si>
+  <si>
+    <t>cARenewalStartegy_END</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>Test Desc</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
+  <si>
+    <t>RenewalType</t>
+  </si>
+  <si>
+    <t>Promotion</t>
+  </si>
+  <si>
+    <t>SKFBJUN16</t>
+  </si>
+  <si>
+    <t>Offer</t>
+  </si>
+  <si>
+    <t>5@5&gt;6@22.45DD</t>
+  </si>
+  <si>
+    <t>CONTINOUS_AUTHORITY</t>
   </si>
 </sst>
 </file>
@@ -677,7 +737,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -696,7 +756,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2777,10 +2840,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2791,6 +2854,8 @@
     <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -2798,6 +2863,8 @@
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -3216,8 +3283,8 @@
       <c r="Q18" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="R18" s="12">
-        <v>38504</v>
+      <c r="R18" s="10" t="s">
+        <v>194</v>
       </c>
       <c r="S18" s="1" t="s">
         <v>1</v>
@@ -3226,6 +3293,166 @@
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>192</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H28" s="12">
+        <v>42564</v>
+      </c>
+      <c r="I28" s="13">
+        <v>42564</v>
+      </c>
+      <c r="J28" s="13">
+        <v>42564</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -3234,6 +3461,8 @@
     <hyperlink ref="C8" r:id="rId2"/>
     <hyperlink ref="C13" r:id="rId3"/>
     <hyperlink ref="C18" r:id="rId4"/>
+    <hyperlink ref="C23" r:id="rId5"/>
+    <hyperlink ref="C28" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>